<commit_message>
Ajout Programme classification et nouvelles données
</commit_message>
<xml_diff>
--- a/Projet-Muse-master/Notes.xlsx
+++ b/Projet-Muse-master/Notes.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FDOS\Geoffrey\Documents\POLYTECH Marseille\4A\Projet Muse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FDOS\Geoffrey\Documents\POLYTECH Marseille\4A\Projet Muse\Project_Muse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B2BB9F-7FB3-4670-B435-B213ED2C9DDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD044ADC-3636-49E6-95FE-C5B40B52DF01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C964CD82-8BC5-49C0-8166-E4C28772A61E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="32">
   <si>
     <t>Tristan</t>
   </si>
@@ -36,98 +36,98 @@
     <t>Geoffrey</t>
   </si>
   <si>
+    <t>Halima</t>
+  </si>
+  <si>
+    <t>FRANCAIS</t>
+  </si>
+  <si>
+    <t>DjaDja</t>
+  </si>
+  <si>
+    <t>louane</t>
+  </si>
+  <si>
+    <t>Nekfeu</t>
+  </si>
+  <si>
+    <t>Angele</t>
+  </si>
+  <si>
+    <t>VIETNAM</t>
+  </si>
+  <si>
+    <t>chung</t>
+  </si>
+  <si>
+    <t>lac-troi</t>
+  </si>
+  <si>
+    <t>my-tam</t>
+  </si>
+  <si>
+    <t>phia</t>
+  </si>
+  <si>
+    <t>CHINE</t>
+  </si>
+  <si>
+    <t>jolin</t>
+  </si>
+  <si>
+    <t>say</t>
+  </si>
+  <si>
+    <t>tizzy</t>
+  </si>
+  <si>
+    <t>vindia</t>
+  </si>
+  <si>
+    <t>MAGHREB</t>
+  </si>
+  <si>
+    <t>mok</t>
+  </si>
+  <si>
+    <t>sanfara</t>
+  </si>
+  <si>
+    <t>dizzy</t>
+  </si>
+  <si>
+    <t>don bigg</t>
+  </si>
+  <si>
+    <t>AFRIQUE</t>
+  </si>
+  <si>
+    <t>abdoulay</t>
+  </si>
+  <si>
+    <t>dtm nani</t>
+  </si>
+  <si>
+    <t>dtm koro</t>
+  </si>
+  <si>
+    <t>rica</t>
+  </si>
+  <si>
+    <t>Sohaib</t>
+  </si>
+  <si>
+    <t>Chaikou</t>
+  </si>
+  <si>
     <t>Mathilde</t>
-  </si>
-  <si>
-    <t>Chaikou</t>
-  </si>
-  <si>
-    <t>Halima</t>
-  </si>
-  <si>
-    <t>Franck</t>
-  </si>
-  <si>
-    <t>FRANCAIS</t>
-  </si>
-  <si>
-    <t>DjaDja</t>
-  </si>
-  <si>
-    <t>louane</t>
-  </si>
-  <si>
-    <t>Nekfeu</t>
-  </si>
-  <si>
-    <t>Angele</t>
-  </si>
-  <si>
-    <t>VIETNAM</t>
-  </si>
-  <si>
-    <t>chung</t>
-  </si>
-  <si>
-    <t>lac-troi</t>
-  </si>
-  <si>
-    <t>my-tam</t>
-  </si>
-  <si>
-    <t>phia</t>
-  </si>
-  <si>
-    <t>CHINE</t>
-  </si>
-  <si>
-    <t>jolin</t>
-  </si>
-  <si>
-    <t>say</t>
-  </si>
-  <si>
-    <t>tizzy</t>
-  </si>
-  <si>
-    <t>vindia</t>
-  </si>
-  <si>
-    <t>MAGHREB</t>
-  </si>
-  <si>
-    <t>mok</t>
-  </si>
-  <si>
-    <t>sanfara</t>
-  </si>
-  <si>
-    <t>dizzy</t>
-  </si>
-  <si>
-    <t>don bigg</t>
-  </si>
-  <si>
-    <t>AFRIQUE</t>
-  </si>
-  <si>
-    <t>abdoulay</t>
-  </si>
-  <si>
-    <t>dtm nani</t>
-  </si>
-  <si>
-    <t>dtm koro</t>
-  </si>
-  <si>
-    <t>rica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +139,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,9 +177,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +500,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,63 +516,87 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>75</v>
       </c>
       <c r="G3">
+        <v>75</v>
+      </c>
+      <c r="H3">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>40</v>
       </c>
       <c r="G4">
+        <v>70</v>
+      </c>
+      <c r="H4" s="2">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
       </c>
       <c r="G5">
+        <v>80</v>
+      </c>
+      <c r="H5">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
       </c>
       <c r="G6">
+        <v>80</v>
+      </c>
+      <c r="H6">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>80</v>
@@ -564,16 +604,25 @@
       <c r="C8">
         <v>85</v>
       </c>
-      <c r="D8">
-        <v>60</v>
+      <c r="D8" s="2">
+        <v>60</v>
+      </c>
+      <c r="E8" s="2">
+        <v>57</v>
+      </c>
+      <c r="F8" s="2">
+        <v>40</v>
       </c>
       <c r="G8">
+        <v>70</v>
+      </c>
+      <c r="H8">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>75</v>
@@ -584,13 +633,22 @@
       <c r="D9">
         <v>65</v>
       </c>
+      <c r="E9">
+        <v>75</v>
+      </c>
+      <c r="F9" s="2">
+        <v>40</v>
+      </c>
       <c r="G9">
+        <v>60</v>
+      </c>
+      <c r="H9">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>65</v>
@@ -598,40 +656,58 @@
       <c r="C10">
         <v>80</v>
       </c>
-      <c r="D10">
-        <v>50</v>
-      </c>
-      <c r="G10">
+      <c r="D10" s="2">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10" s="2">
+        <v>50</v>
+      </c>
+      <c r="H10">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>65</v>
       </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-      <c r="D11">
-        <v>60</v>
-      </c>
-      <c r="G11">
+      <c r="C11" s="2">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2">
+        <v>60</v>
+      </c>
+      <c r="E11" s="2">
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11" s="2">
+        <v>40</v>
+      </c>
+      <c r="H11">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2">
         <v>55</v>
       </c>
       <c r="C13">
@@ -640,30 +716,48 @@
       <c r="D13">
         <v>65</v>
       </c>
-      <c r="G13">
+      <c r="E13">
+        <v>65</v>
+      </c>
+      <c r="F13">
+        <v>55</v>
+      </c>
+      <c r="G13" s="2">
+        <v>30</v>
+      </c>
+      <c r="H13">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2">
         <v>40</v>
       </c>
       <c r="C14">
         <v>75</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>40</v>
       </c>
+      <c r="E14" s="2">
+        <v>50</v>
+      </c>
+      <c r="F14" s="2">
+        <v>50</v>
+      </c>
       <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>75</v>
@@ -674,79 +768,115 @@
       <c r="D15">
         <v>75</v>
       </c>
-      <c r="G15">
+      <c r="E15" s="3">
+        <v>60</v>
+      </c>
+      <c r="F15">
+        <v>60</v>
+      </c>
+      <c r="G15" s="2">
+        <v>50</v>
+      </c>
+      <c r="H15">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>75</v>
+      </c>
+      <c r="C16">
+        <v>80</v>
+      </c>
+      <c r="D16">
+        <v>70</v>
+      </c>
+      <c r="E16">
+        <v>76</v>
+      </c>
+      <c r="F16">
+        <v>60</v>
+      </c>
+      <c r="G16">
+        <v>70</v>
+      </c>
+      <c r="H16">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2">
+        <v>60</v>
+      </c>
+      <c r="C18" s="3">
+        <v>60</v>
+      </c>
+      <c r="D18">
+        <v>75</v>
+      </c>
+      <c r="E18" s="3">
+        <v>60</v>
+      </c>
+      <c r="F18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
-        <v>75</v>
-      </c>
-      <c r="C16">
-        <v>80</v>
-      </c>
-      <c r="D16">
-        <v>70</v>
-      </c>
-      <c r="G16">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B19">
+        <v>75</v>
+      </c>
+      <c r="C19" s="2">
+        <v>35</v>
+      </c>
+      <c r="D19">
+        <v>70</v>
+      </c>
+      <c r="E19" s="4">
+        <v>52</v>
+      </c>
+      <c r="F19" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B20" s="2">
+        <v>55</v>
+      </c>
+      <c r="C20" s="2">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>75</v>
+      </c>
+      <c r="E20" s="2">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
-        <v>60</v>
-      </c>
-      <c r="C18">
-        <v>60</v>
-      </c>
-      <c r="D18">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>75</v>
-      </c>
-      <c r="C19">
-        <v>35</v>
-      </c>
-      <c r="D19">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>55</v>
-      </c>
-      <c r="C20">
-        <v>30</v>
-      </c>
-      <c r="D20">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>55</v>
       </c>
       <c r="C21">
@@ -755,51 +885,69 @@
       <c r="D21">
         <v>70</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2">
+        <v>20</v>
+      </c>
+      <c r="F21" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <v>70</v>
+      </c>
+      <c r="D23" s="2">
+        <v>45</v>
+      </c>
+      <c r="E23" s="2">
+        <v>20</v>
+      </c>
+      <c r="G23" s="2">
+        <v>40</v>
+      </c>
+      <c r="H23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23">
-        <v>35</v>
-      </c>
-      <c r="C23">
-        <v>70</v>
-      </c>
-      <c r="D23">
-        <v>45</v>
-      </c>
-      <c r="G23">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
       <c r="B24">
         <v>50</v>
       </c>
       <c r="C24">
         <v>60</v>
       </c>
-      <c r="D24">
-        <v>60</v>
+      <c r="D24" s="2">
+        <v>60</v>
+      </c>
+      <c r="E24" s="2">
+        <v>50</v>
       </c>
       <c r="G24">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="H24">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2">
         <v>45</v>
       </c>
       <c r="C25">
@@ -808,24 +956,36 @@
       <c r="D25">
         <v>65</v>
       </c>
+      <c r="E25">
+        <v>55</v>
+      </c>
       <c r="G25">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="H25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2">
         <v>30</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>40</v>
       </c>
-      <c r="D26">
-        <v>60</v>
+      <c r="D26" s="2">
+        <v>60</v>
+      </c>
+      <c r="E26" s="2">
+        <v>26</v>
       </c>
       <c r="G26">
+        <v>60</v>
+      </c>
+      <c r="H26">
         <v>60</v>
       </c>
     </row>

</xml_diff>